<commit_message>
another changes in xl file
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="10">
   <si>
     <t>Sunday</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>2 . Git</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -1194,7 +1197,7 @@
         <xdr:cNvPr id="3" name="Picture 2" descr="Photo collage of word: Winter" title="Header Winter">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1248,7 +1251,7 @@
         <xdr:cNvPr id="4" name="Picture 3" descr="Photo collage of word: Fall" title="Header Fall">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0900-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0900-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1302,7 +1305,7 @@
         <xdr:cNvPr id="4" name="Picture 3" descr="Photo collage of word: Fall" title="Header Fall">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0A00-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1356,7 +1359,7 @@
         <xdr:cNvPr id="3" name="Picture 2" descr="Photo collage of word: Winter" title="Header Winter">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0B00-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1410,7 +1413,7 @@
         <xdr:cNvPr id="3" name="Picture 2" descr="Photo collage of word: Winter" title="Header Winter">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1464,7 +1467,7 @@
         <xdr:cNvPr id="2" name="Picture 1" descr="Photo collage of word: Spring" title="Header Spring">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1518,7 +1521,7 @@
         <xdr:cNvPr id="4" name="Picture 3" descr="Photo collage of word: Spring" title="Header Spring">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1572,7 +1575,7 @@
         <xdr:cNvPr id="4" name="Picture 3" descr="Photo collage of word: Spring" title="Header Spring">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1626,7 +1629,7 @@
         <xdr:cNvPr id="3" name="Picture 2" descr="Photo collage of word: Summer" title="Header Summer">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1680,7 +1683,7 @@
         <xdr:cNvPr id="4" name="Picture 3" descr="Photo collage of word: Summer" title="Header Summer">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1734,7 +1737,7 @@
         <xdr:cNvPr id="4" name="Picture 3" descr="Photo collage of word: Summer" title="Header Summer">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1788,7 +1791,7 @@
         <xdr:cNvPr id="3" name="Picture 2" descr="Photo collage of word: Fall" title="Header Fall">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0800-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0800-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3887,7 +3890,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3984,7 +3987,9 @@
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
       <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
+      <c r="F5" s="30" t="s">
+        <v>9</v>
+      </c>
       <c r="G5" s="30"/>
       <c r="H5" s="30"/>
     </row>
@@ -5707,23 +5712,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e39e7e9e36de66d473ce04bb4ab2dbb8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="19dc5994665da46609c24125788630d8" ns2:_="" ns3:_="">
     <xsd:import namespace="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
@@ -5928,25 +5916,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B8A745B-63BA-4F9A-A6E5-C457B3F40DFD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6B20271-DBF4-4EBA-824D-0E74CCAA174D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CD1B5DC0-C7DA-4FC0-BFE2-1D1407D5E729}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5963,4 +5950,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6B20271-DBF4-4EBA-824D-0E74CCAA174D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B8A745B-63BA-4F9A-A6E5-C457B3F40DFD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>